<commit_message>
Upando exercícios de normalização de dados
</commit_message>
<xml_diff>
--- a/normalization/list-01/question-3/question3.xlsx
+++ b/normalization/list-01/question-3/question3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliente\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliente\Documents\ws-database\normalization\list-01\question-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,12 +77,6 @@
     <t>{idPedido, codProduto} ~=&gt; dataPedido</t>
   </si>
   <si>
-    <t>codProduto -&gt; codProduto</t>
-  </si>
-  <si>
-    <t>{idPedido, codProduto} ~=&gt; codProduto</t>
-  </si>
-  <si>
     <t>codProduto -&gt; codCategoria</t>
   </si>
   <si>
@@ -108,6 +102,12 @@
   </si>
   <si>
     <t>codProduto -&gt; valorUnitario</t>
+  </si>
+  <si>
+    <t>{idPedido, codProduto} ~=&gt; nomeProduto</t>
+  </si>
+  <si>
+    <t>codProduto -&gt; nomeProduto</t>
   </si>
 </sst>
 </file>
@@ -220,11 +220,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,16 +539,16 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -711,100 +711,100 @@
         <v>14</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="5"/>
       <c r="G12" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="G14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="B16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="B21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>